<commit_message>
thêm export import + quyền
</commit_message>
<xml_diff>
--- a/beautify_api/8.0.0/aspnet-core/src/BanHangBeautify.Web.Host/wwwroot/ExcelTemplate/KhachHang_Export_Template.xlsx
+++ b/beautify_api/8.0.0/aspnet-core/src/BanHangBeautify.Web.Host/wwwroot/ExcelTemplate/KhachHang_Export_Template.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\code-manhld-github\beautify_app_flutter\beautify_api\8.0.0\aspnet-core\src\BanHangBeautify.Web.Host\wwwroot\ExcelTemplate\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13740"/>
   </bookViews>
@@ -10,8 +15,8 @@
     <sheet name="DanhSach" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="124519"/>
-  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -101,8 +106,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="5">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -205,7 +210,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -215,9 +220,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -231,9 +233,6 @@
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -243,6 +242,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="22" fontId="3" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -305,7 +307,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -340,7 +342,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -517,29 +519,29 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AT7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:DD14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A2" sqref="A2"/>
-      <selection pane="bottomLeft" activeCell="E14" sqref="E14"/>
+      <selection pane="bottomLeft" activeCell="F16" sqref="F16:F17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="7" style="1" customWidth="1"/>
     <col min="2" max="2" width="16" style="1" customWidth="1"/>
     <col min="3" max="3" width="30.140625" style="2" customWidth="1"/>
     <col min="4" max="4" width="20.85546875" style="2" customWidth="1"/>
-    <col min="5" max="5" width="40.7109375" style="6" customWidth="1"/>
+    <col min="5" max="5" width="40.7109375" style="5" customWidth="1"/>
     <col min="6" max="6" width="21.7109375" style="1" customWidth="1"/>
     <col min="7" max="7" width="13.85546875" style="2" customWidth="1"/>
     <col min="8" max="8" width="18.5703125" style="2" customWidth="1"/>
@@ -547,11 +549,11 @@
     <col min="10" max="10" width="23.7109375" style="2" customWidth="1"/>
     <col min="11" max="11" width="25.28515625" style="2" customWidth="1"/>
     <col min="12" max="12" width="24" style="2" customWidth="1"/>
-    <col min="13" max="13" width="19.28515625" style="8" customWidth="1"/>
+    <col min="13" max="13" width="19.28515625" style="7" customWidth="1"/>
     <col min="14" max="14" width="24" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:46" ht="15" hidden="1" customHeight="1">
+    <row r="1" spans="1:108" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
@@ -573,64 +575,66 @@
       <c r="I1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="M1" s="8" t="s">
+      <c r="M1" s="7" t="s">
         <v>0</v>
       </c>
       <c r="N1" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:46" ht="41.25" customHeight="1">
-      <c r="B2" s="9" t="s">
+    <row r="2" spans="1:108" ht="41.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A2" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
-      <c r="F2" s="9"/>
-      <c r="G2" s="9"/>
-      <c r="H2" s="4"/>
-      <c r="I2" s="4"/>
-      <c r="J2" s="4"/>
-      <c r="K2" s="4"/>
-      <c r="L2" s="4"/>
+      <c r="B2" s="12"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
+      <c r="G2" s="12"/>
+      <c r="H2" s="12"/>
+      <c r="I2" s="12"/>
+      <c r="J2" s="12"/>
+      <c r="K2" s="12"/>
+      <c r="L2" s="12"/>
+      <c r="M2" s="12"/>
     </row>
-    <row r="3" spans="1:46">
-      <c r="N3" s="11"/>
-      <c r="O3" s="12"/>
-      <c r="P3" s="12"/>
-      <c r="Q3" s="12"/>
-      <c r="R3" s="12"/>
-      <c r="S3" s="12"/>
-      <c r="T3" s="12"/>
-      <c r="U3" s="12"/>
-      <c r="V3" s="12"/>
-      <c r="W3" s="12"/>
-      <c r="X3" s="12"/>
-      <c r="Y3" s="12"/>
-      <c r="Z3" s="12"/>
-      <c r="AA3" s="12"/>
-      <c r="AB3" s="12"/>
-      <c r="AC3" s="12"/>
-      <c r="AD3" s="12"/>
-      <c r="AE3" s="12"/>
-      <c r="AF3" s="12"/>
-      <c r="AG3" s="12"/>
-      <c r="AH3" s="12"/>
-      <c r="AI3" s="12"/>
-      <c r="AJ3" s="12"/>
-      <c r="AK3" s="12"/>
-      <c r="AL3" s="12"/>
-      <c r="AM3" s="12"/>
-      <c r="AN3" s="12"/>
-      <c r="AO3" s="12"/>
-      <c r="AP3" s="12"/>
-      <c r="AQ3" s="12"/>
-      <c r="AR3" s="12"/>
-      <c r="AS3" s="12"/>
-      <c r="AT3" s="12"/>
+    <row r="3" spans="1:108" x14ac:dyDescent="0.25">
+      <c r="N3" s="9"/>
+      <c r="O3" s="10"/>
+      <c r="P3" s="10"/>
+      <c r="Q3" s="10"/>
+      <c r="R3" s="10"/>
+      <c r="S3" s="10"/>
+      <c r="T3" s="10"/>
+      <c r="U3" s="10"/>
+      <c r="V3" s="10"/>
+      <c r="W3" s="10"/>
+      <c r="X3" s="10"/>
+      <c r="Y3" s="10"/>
+      <c r="Z3" s="10"/>
+      <c r="AA3" s="10"/>
+      <c r="AB3" s="10"/>
+      <c r="AC3" s="10"/>
+      <c r="AD3" s="10"/>
+      <c r="AE3" s="10"/>
+      <c r="AF3" s="10"/>
+      <c r="AG3" s="10"/>
+      <c r="AH3" s="10"/>
+      <c r="AI3" s="10"/>
+      <c r="AJ3" s="10"/>
+      <c r="AK3" s="10"/>
+      <c r="AL3" s="10"/>
+      <c r="AM3" s="10"/>
+      <c r="AN3" s="10"/>
+      <c r="AO3" s="10"/>
+      <c r="AP3" s="10"/>
+      <c r="AQ3" s="10"/>
+      <c r="AR3" s="10"/>
+      <c r="AS3" s="10"/>
+      <c r="AT3" s="10"/>
     </row>
-    <row r="4" spans="1:46" s="5" customFormat="1" ht="30.75" customHeight="1">
+    <row r="4" spans="1:108" s="4" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>9</v>
       </c>
@@ -643,7 +647,7 @@
       <c r="D4" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="E4" s="7" t="s">
+      <c r="E4" s="6" t="s">
         <v>11</v>
       </c>
       <c r="F4" s="3" t="s">
@@ -667,151 +671,1078 @@
       <c r="L4" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="M4" s="13" t="s">
+      <c r="M4" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="N4" s="10"/>
-      <c r="O4" s="10"/>
-      <c r="P4" s="10"/>
-      <c r="Q4" s="10"/>
-      <c r="R4" s="10"/>
-      <c r="S4" s="10"/>
-      <c r="T4" s="10"/>
-      <c r="U4" s="10"/>
-      <c r="V4" s="10"/>
-      <c r="W4" s="10"/>
-      <c r="X4" s="10"/>
-      <c r="Y4" s="10"/>
-      <c r="Z4" s="10"/>
-      <c r="AA4" s="10"/>
-      <c r="AB4" s="10"/>
-      <c r="AC4" s="10"/>
-      <c r="AD4" s="10"/>
-      <c r="AE4" s="10"/>
-      <c r="AF4" s="10"/>
-      <c r="AG4" s="10"/>
-      <c r="AH4" s="10"/>
-      <c r="AI4" s="10"/>
-      <c r="AJ4" s="10"/>
-      <c r="AK4" s="10"/>
-      <c r="AL4" s="10"/>
-      <c r="AM4" s="10"/>
-      <c r="AN4" s="10"/>
-      <c r="AO4" s="10"/>
-      <c r="AP4" s="10"/>
-      <c r="AQ4" s="10"/>
-      <c r="AR4" s="10"/>
-      <c r="AS4" s="10"/>
-      <c r="AT4" s="10"/>
+      <c r="N4" s="8"/>
+      <c r="O4" s="8"/>
+      <c r="P4" s="8"/>
+      <c r="Q4" s="8"/>
+      <c r="R4" s="8"/>
+      <c r="S4" s="8"/>
+      <c r="T4" s="8"/>
+      <c r="U4" s="8"/>
+      <c r="V4" s="8"/>
+      <c r="W4" s="8"/>
+      <c r="X4" s="8"/>
+      <c r="Y4" s="8"/>
+      <c r="Z4" s="8"/>
+      <c r="AA4" s="8"/>
+      <c r="AB4" s="8"/>
+      <c r="AC4" s="8"/>
+      <c r="AD4" s="8"/>
+      <c r="AE4" s="8"/>
+      <c r="AF4" s="8"/>
+      <c r="AG4" s="8"/>
+      <c r="AH4" s="8"/>
+      <c r="AI4" s="8"/>
+      <c r="AJ4" s="8"/>
+      <c r="AK4" s="8"/>
+      <c r="AL4" s="8"/>
+      <c r="AM4" s="8"/>
+      <c r="AN4" s="8"/>
+      <c r="AO4" s="8"/>
+      <c r="AP4" s="8"/>
+      <c r="AQ4" s="8"/>
+      <c r="AR4" s="8"/>
+      <c r="AS4" s="8"/>
+      <c r="AT4" s="8"/>
+      <c r="AU4" s="8"/>
+      <c r="AV4" s="8"/>
+      <c r="AW4" s="8"/>
+      <c r="AX4" s="8"/>
+      <c r="AY4" s="8"/>
+      <c r="AZ4" s="8"/>
+      <c r="BA4" s="8"/>
+      <c r="BB4" s="8"/>
+      <c r="BC4" s="8"/>
+      <c r="BD4" s="8"/>
+      <c r="BE4" s="8"/>
+      <c r="BF4" s="8"/>
+      <c r="BG4" s="8"/>
+      <c r="BH4" s="8"/>
+      <c r="BI4" s="8"/>
+      <c r="BJ4" s="8"/>
+      <c r="BK4" s="8"/>
+      <c r="BL4" s="8"/>
+      <c r="BM4" s="8"/>
+      <c r="BN4" s="8"/>
+      <c r="BO4" s="8"/>
+      <c r="BP4" s="8"/>
+      <c r="BQ4" s="8"/>
+      <c r="BR4" s="8"/>
+      <c r="BS4" s="8"/>
+      <c r="BT4" s="8"/>
+      <c r="BU4" s="8"/>
+      <c r="BV4" s="8"/>
+      <c r="BW4" s="8"/>
+      <c r="BX4" s="8"/>
+      <c r="BY4" s="8"/>
+      <c r="BZ4" s="8"/>
+      <c r="CA4" s="8"/>
+      <c r="CB4" s="8"/>
+      <c r="CC4" s="8"/>
+      <c r="CD4" s="8"/>
+      <c r="CE4" s="8"/>
+      <c r="CF4" s="8"/>
+      <c r="CG4" s="8"/>
+      <c r="CH4" s="8"/>
+      <c r="CI4" s="8"/>
+      <c r="CJ4" s="8"/>
+      <c r="CK4" s="8"/>
+      <c r="CL4" s="8"/>
+      <c r="CM4" s="8"/>
+      <c r="CN4" s="8"/>
+      <c r="CO4" s="8"/>
+      <c r="CP4" s="8"/>
+      <c r="CQ4" s="8"/>
+      <c r="CR4" s="8"/>
+      <c r="CS4" s="8"/>
+      <c r="CT4" s="8"/>
+      <c r="CU4" s="8"/>
+      <c r="CV4" s="8"/>
+      <c r="CW4" s="8"/>
+      <c r="CX4" s="8"/>
+      <c r="CY4" s="8"/>
+      <c r="CZ4" s="8"/>
+      <c r="DA4" s="8"/>
+      <c r="DB4" s="8"/>
+      <c r="DC4" s="8"/>
+      <c r="DD4" s="8"/>
     </row>
-    <row r="5" spans="1:46">
-      <c r="N5" s="11"/>
-      <c r="O5" s="12"/>
-      <c r="P5" s="12"/>
-      <c r="Q5" s="12"/>
-      <c r="R5" s="12"/>
-      <c r="S5" s="12"/>
-      <c r="T5" s="12"/>
-      <c r="U5" s="12"/>
-      <c r="V5" s="12"/>
-      <c r="W5" s="12"/>
-      <c r="X5" s="12"/>
-      <c r="Y5" s="12"/>
-      <c r="Z5" s="12"/>
-      <c r="AA5" s="12"/>
-      <c r="AB5" s="12"/>
-      <c r="AC5" s="12"/>
-      <c r="AD5" s="12"/>
-      <c r="AE5" s="12"/>
-      <c r="AF5" s="12"/>
-      <c r="AG5" s="12"/>
-      <c r="AH5" s="12"/>
-      <c r="AI5" s="12"/>
-      <c r="AJ5" s="12"/>
-      <c r="AK5" s="12"/>
-      <c r="AL5" s="12"/>
-      <c r="AM5" s="12"/>
-      <c r="AN5" s="12"/>
-      <c r="AO5" s="12"/>
-      <c r="AP5" s="12"/>
-      <c r="AQ5" s="12"/>
-      <c r="AR5" s="12"/>
-      <c r="AS5" s="12"/>
-      <c r="AT5" s="12"/>
+    <row r="5" spans="1:108" x14ac:dyDescent="0.25">
+      <c r="N5" s="9"/>
+      <c r="O5" s="10"/>
+      <c r="P5" s="10"/>
+      <c r="Q5" s="10"/>
+      <c r="R5" s="10"/>
+      <c r="S5" s="10"/>
+      <c r="T5" s="10"/>
+      <c r="U5" s="10"/>
+      <c r="V5" s="10"/>
+      <c r="W5" s="10"/>
+      <c r="X5" s="10"/>
+      <c r="Y5" s="10"/>
+      <c r="Z5" s="10"/>
+      <c r="AA5" s="10"/>
+      <c r="AB5" s="10"/>
+      <c r="AC5" s="10"/>
+      <c r="AD5" s="10"/>
+      <c r="AE5" s="10"/>
+      <c r="AF5" s="10"/>
+      <c r="AG5" s="10"/>
+      <c r="AH5" s="10"/>
+      <c r="AI5" s="10"/>
+      <c r="AJ5" s="10"/>
+      <c r="AK5" s="10"/>
+      <c r="AL5" s="10"/>
+      <c r="AM5" s="10"/>
+      <c r="AN5" s="10"/>
+      <c r="AO5" s="10"/>
+      <c r="AP5" s="10"/>
+      <c r="AQ5" s="10"/>
+      <c r="AR5" s="10"/>
+      <c r="AS5" s="10"/>
+      <c r="AT5" s="10"/>
+      <c r="AU5" s="10"/>
+      <c r="AV5" s="10"/>
+      <c r="AW5" s="10"/>
+      <c r="AX5" s="10"/>
+      <c r="AY5" s="10"/>
+      <c r="AZ5" s="10"/>
+      <c r="BA5" s="10"/>
+      <c r="BB5" s="10"/>
+      <c r="BC5" s="10"/>
+      <c r="BD5" s="10"/>
+      <c r="BE5" s="10"/>
+      <c r="BF5" s="10"/>
+      <c r="BG5" s="10"/>
+      <c r="BH5" s="10"/>
+      <c r="BI5" s="10"/>
+      <c r="BJ5" s="10"/>
+      <c r="BK5" s="10"/>
+      <c r="BL5" s="10"/>
+      <c r="BM5" s="10"/>
+      <c r="BN5" s="10"/>
+      <c r="BO5" s="10"/>
+      <c r="BP5" s="10"/>
+      <c r="BQ5" s="10"/>
+      <c r="BR5" s="10"/>
+      <c r="BS5" s="10"/>
+      <c r="BT5" s="10"/>
+      <c r="BU5" s="10"/>
+      <c r="BV5" s="10"/>
+      <c r="BW5" s="10"/>
+      <c r="BX5" s="10"/>
+      <c r="BY5" s="10"/>
+      <c r="BZ5" s="10"/>
+      <c r="CA5" s="10"/>
+      <c r="CB5" s="10"/>
+      <c r="CC5" s="10"/>
+      <c r="CD5" s="10"/>
+      <c r="CE5" s="10"/>
+      <c r="CF5" s="10"/>
+      <c r="CG5" s="10"/>
+      <c r="CH5" s="10"/>
+      <c r="CI5" s="10"/>
+      <c r="CJ5" s="10"/>
+      <c r="CK5" s="10"/>
+      <c r="CL5" s="10"/>
+      <c r="CM5" s="10"/>
+      <c r="CN5" s="10"/>
+      <c r="CO5" s="10"/>
+      <c r="CP5" s="10"/>
+      <c r="CQ5" s="10"/>
+      <c r="CR5" s="10"/>
+      <c r="CS5" s="10"/>
+      <c r="CT5" s="10"/>
+      <c r="CU5" s="10"/>
+      <c r="CV5" s="10"/>
+      <c r="CW5" s="10"/>
+      <c r="CX5" s="10"/>
+      <c r="CY5" s="10"/>
+      <c r="CZ5" s="10"/>
+      <c r="DA5" s="10"/>
+      <c r="DB5" s="10"/>
+      <c r="DC5" s="10"/>
+      <c r="DD5" s="10"/>
     </row>
-    <row r="6" spans="1:46">
-      <c r="N6" s="11"/>
-      <c r="O6" s="12"/>
-      <c r="P6" s="12"/>
-      <c r="Q6" s="12"/>
-      <c r="R6" s="12"/>
-      <c r="S6" s="12"/>
-      <c r="T6" s="12"/>
-      <c r="U6" s="12"/>
-      <c r="V6" s="12"/>
-      <c r="W6" s="12"/>
-      <c r="X6" s="12"/>
-      <c r="Y6" s="12"/>
-      <c r="Z6" s="12"/>
-      <c r="AA6" s="12"/>
-      <c r="AB6" s="12"/>
-      <c r="AC6" s="12"/>
-      <c r="AD6" s="12"/>
-      <c r="AE6" s="12"/>
-      <c r="AF6" s="12"/>
-      <c r="AG6" s="12"/>
-      <c r="AH6" s="12"/>
-      <c r="AI6" s="12"/>
-      <c r="AJ6" s="12"/>
-      <c r="AK6" s="12"/>
-      <c r="AL6" s="12"/>
-      <c r="AM6" s="12"/>
-      <c r="AN6" s="12"/>
-      <c r="AO6" s="12"/>
-      <c r="AP6" s="12"/>
-      <c r="AQ6" s="12"/>
-      <c r="AR6" s="12"/>
-      <c r="AS6" s="12"/>
-      <c r="AT6" s="12"/>
+    <row r="6" spans="1:108" x14ac:dyDescent="0.25">
+      <c r="N6" s="9"/>
+      <c r="O6" s="10"/>
+      <c r="P6" s="10"/>
+      <c r="Q6" s="10"/>
+      <c r="R6" s="10"/>
+      <c r="S6" s="10"/>
+      <c r="T6" s="10"/>
+      <c r="U6" s="10"/>
+      <c r="V6" s="10"/>
+      <c r="W6" s="10"/>
+      <c r="X6" s="10"/>
+      <c r="Y6" s="10"/>
+      <c r="Z6" s="10"/>
+      <c r="AA6" s="10"/>
+      <c r="AB6" s="10"/>
+      <c r="AC6" s="10"/>
+      <c r="AD6" s="10"/>
+      <c r="AE6" s="10"/>
+      <c r="AF6" s="10"/>
+      <c r="AG6" s="10"/>
+      <c r="AH6" s="10"/>
+      <c r="AI6" s="10"/>
+      <c r="AJ6" s="10"/>
+      <c r="AK6" s="10"/>
+      <c r="AL6" s="10"/>
+      <c r="AM6" s="10"/>
+      <c r="AN6" s="10"/>
+      <c r="AO6" s="10"/>
+      <c r="AP6" s="10"/>
+      <c r="AQ6" s="10"/>
+      <c r="AR6" s="10"/>
+      <c r="AS6" s="10"/>
+      <c r="AT6" s="10"/>
+      <c r="AU6" s="10"/>
+      <c r="AV6" s="10"/>
+      <c r="AW6" s="10"/>
+      <c r="AX6" s="10"/>
+      <c r="AY6" s="10"/>
+      <c r="AZ6" s="10"/>
+      <c r="BA6" s="10"/>
+      <c r="BB6" s="10"/>
+      <c r="BC6" s="10"/>
+      <c r="BD6" s="10"/>
+      <c r="BE6" s="10"/>
+      <c r="BF6" s="10"/>
+      <c r="BG6" s="10"/>
+      <c r="BH6" s="10"/>
+      <c r="BI6" s="10"/>
+      <c r="BJ6" s="10"/>
+      <c r="BK6" s="10"/>
+      <c r="BL6" s="10"/>
+      <c r="BM6" s="10"/>
+      <c r="BN6" s="10"/>
+      <c r="BO6" s="10"/>
+      <c r="BP6" s="10"/>
+      <c r="BQ6" s="10"/>
+      <c r="BR6" s="10"/>
+      <c r="BS6" s="10"/>
+      <c r="BT6" s="10"/>
+      <c r="BU6" s="10"/>
+      <c r="BV6" s="10"/>
+      <c r="BW6" s="10"/>
+      <c r="BX6" s="10"/>
+      <c r="BY6" s="10"/>
+      <c r="BZ6" s="10"/>
+      <c r="CA6" s="10"/>
+      <c r="CB6" s="10"/>
+      <c r="CC6" s="10"/>
+      <c r="CD6" s="10"/>
+      <c r="CE6" s="10"/>
+      <c r="CF6" s="10"/>
+      <c r="CG6" s="10"/>
+      <c r="CH6" s="10"/>
+      <c r="CI6" s="10"/>
+      <c r="CJ6" s="10"/>
+      <c r="CK6" s="10"/>
+      <c r="CL6" s="10"/>
+      <c r="CM6" s="10"/>
+      <c r="CN6" s="10"/>
+      <c r="CO6" s="10"/>
+      <c r="CP6" s="10"/>
+      <c r="CQ6" s="10"/>
+      <c r="CR6" s="10"/>
+      <c r="CS6" s="10"/>
+      <c r="CT6" s="10"/>
+      <c r="CU6" s="10"/>
+      <c r="CV6" s="10"/>
+      <c r="CW6" s="10"/>
+      <c r="CX6" s="10"/>
+      <c r="CY6" s="10"/>
+      <c r="CZ6" s="10"/>
+      <c r="DA6" s="10"/>
+      <c r="DB6" s="10"/>
+      <c r="DC6" s="10"/>
+      <c r="DD6" s="10"/>
     </row>
-    <row r="7" spans="1:46">
-      <c r="N7" s="11"/>
-      <c r="O7" s="12"/>
-      <c r="P7" s="12"/>
-      <c r="Q7" s="12"/>
-      <c r="R7" s="12"/>
-      <c r="S7" s="12"/>
-      <c r="T7" s="12"/>
-      <c r="U7" s="12"/>
-      <c r="V7" s="12"/>
-      <c r="W7" s="12"/>
-      <c r="X7" s="12"/>
-      <c r="Y7" s="12"/>
-      <c r="Z7" s="12"/>
-      <c r="AA7" s="12"/>
-      <c r="AB7" s="12"/>
-      <c r="AC7" s="12"/>
-      <c r="AD7" s="12"/>
-      <c r="AE7" s="12"/>
-      <c r="AF7" s="12"/>
-      <c r="AG7" s="12"/>
-      <c r="AH7" s="12"/>
-      <c r="AI7" s="12"/>
-      <c r="AJ7" s="12"/>
-      <c r="AK7" s="12"/>
-      <c r="AL7" s="12"/>
-      <c r="AM7" s="12"/>
-      <c r="AN7" s="12"/>
-      <c r="AO7" s="12"/>
-      <c r="AP7" s="12"/>
-      <c r="AQ7" s="12"/>
-      <c r="AR7" s="12"/>
-      <c r="AS7" s="12"/>
-      <c r="AT7" s="12"/>
+    <row r="7" spans="1:108" x14ac:dyDescent="0.25">
+      <c r="N7" s="9"/>
+      <c r="O7" s="10"/>
+      <c r="P7" s="10"/>
+      <c r="Q7" s="10"/>
+      <c r="R7" s="10"/>
+      <c r="S7" s="10"/>
+      <c r="T7" s="10"/>
+      <c r="U7" s="10"/>
+      <c r="V7" s="10"/>
+      <c r="W7" s="10"/>
+      <c r="X7" s="10"/>
+      <c r="Y7" s="10"/>
+      <c r="Z7" s="10"/>
+      <c r="AA7" s="10"/>
+      <c r="AB7" s="10"/>
+      <c r="AC7" s="10"/>
+      <c r="AD7" s="10"/>
+      <c r="AE7" s="10"/>
+      <c r="AF7" s="10"/>
+      <c r="AG7" s="10"/>
+      <c r="AH7" s="10"/>
+      <c r="AI7" s="10"/>
+      <c r="AJ7" s="10"/>
+      <c r="AK7" s="10"/>
+      <c r="AL7" s="10"/>
+      <c r="AM7" s="10"/>
+      <c r="AN7" s="10"/>
+      <c r="AO7" s="10"/>
+      <c r="AP7" s="10"/>
+      <c r="AQ7" s="10"/>
+      <c r="AR7" s="10"/>
+      <c r="AS7" s="10"/>
+      <c r="AT7" s="10"/>
+      <c r="AU7" s="10"/>
+      <c r="AV7" s="10"/>
+      <c r="AW7" s="10"/>
+      <c r="AX7" s="10"/>
+      <c r="AY7" s="10"/>
+      <c r="AZ7" s="10"/>
+      <c r="BA7" s="10"/>
+      <c r="BB7" s="10"/>
+      <c r="BC7" s="10"/>
+      <c r="BD7" s="10"/>
+      <c r="BE7" s="10"/>
+      <c r="BF7" s="10"/>
+      <c r="BG7" s="10"/>
+      <c r="BH7" s="10"/>
+      <c r="BI7" s="10"/>
+      <c r="BJ7" s="10"/>
+      <c r="BK7" s="10"/>
+      <c r="BL7" s="10"/>
+      <c r="BM7" s="10"/>
+      <c r="BN7" s="10"/>
+      <c r="BO7" s="10"/>
+      <c r="BP7" s="10"/>
+      <c r="BQ7" s="10"/>
+      <c r="BR7" s="10"/>
+      <c r="BS7" s="10"/>
+      <c r="BT7" s="10"/>
+      <c r="BU7" s="10"/>
+      <c r="BV7" s="10"/>
+      <c r="BW7" s="10"/>
+      <c r="BX7" s="10"/>
+      <c r="BY7" s="10"/>
+      <c r="BZ7" s="10"/>
+      <c r="CA7" s="10"/>
+      <c r="CB7" s="10"/>
+      <c r="CC7" s="10"/>
+      <c r="CD7" s="10"/>
+      <c r="CE7" s="10"/>
+      <c r="CF7" s="10"/>
+      <c r="CG7" s="10"/>
+      <c r="CH7" s="10"/>
+      <c r="CI7" s="10"/>
+      <c r="CJ7" s="10"/>
+      <c r="CK7" s="10"/>
+      <c r="CL7" s="10"/>
+      <c r="CM7" s="10"/>
+      <c r="CN7" s="10"/>
+      <c r="CO7" s="10"/>
+      <c r="CP7" s="10"/>
+      <c r="CQ7" s="10"/>
+      <c r="CR7" s="10"/>
+      <c r="CS7" s="10"/>
+      <c r="CT7" s="10"/>
+      <c r="CU7" s="10"/>
+      <c r="CV7" s="10"/>
+      <c r="CW7" s="10"/>
+      <c r="CX7" s="10"/>
+      <c r="CY7" s="10"/>
+      <c r="CZ7" s="10"/>
+      <c r="DA7" s="10"/>
+      <c r="DB7" s="10"/>
+      <c r="DC7" s="10"/>
+      <c r="DD7" s="10"/>
+    </row>
+    <row r="8" spans="1:108" x14ac:dyDescent="0.25">
+      <c r="N8" s="9"/>
+      <c r="O8" s="10"/>
+      <c r="P8" s="10"/>
+      <c r="Q8" s="10"/>
+      <c r="R8" s="10"/>
+      <c r="S8" s="10"/>
+      <c r="T8" s="10"/>
+      <c r="U8" s="10"/>
+      <c r="V8" s="10"/>
+      <c r="W8" s="10"/>
+      <c r="X8" s="10"/>
+      <c r="Y8" s="10"/>
+      <c r="Z8" s="10"/>
+      <c r="AA8" s="10"/>
+      <c r="AB8" s="10"/>
+      <c r="AC8" s="10"/>
+      <c r="AD8" s="10"/>
+      <c r="AE8" s="10"/>
+      <c r="AF8" s="10"/>
+      <c r="AG8" s="10"/>
+      <c r="AH8" s="10"/>
+      <c r="AI8" s="10"/>
+      <c r="AJ8" s="10"/>
+      <c r="AK8" s="10"/>
+      <c r="AL8" s="10"/>
+      <c r="AM8" s="10"/>
+      <c r="AN8" s="10"/>
+      <c r="AO8" s="10"/>
+      <c r="AP8" s="10"/>
+      <c r="AQ8" s="10"/>
+      <c r="AR8" s="10"/>
+      <c r="AS8" s="10"/>
+      <c r="AT8" s="10"/>
+      <c r="AU8" s="10"/>
+      <c r="AV8" s="10"/>
+      <c r="AW8" s="10"/>
+      <c r="AX8" s="10"/>
+      <c r="AY8" s="10"/>
+      <c r="AZ8" s="10"/>
+      <c r="BA8" s="10"/>
+      <c r="BB8" s="10"/>
+      <c r="BC8" s="10"/>
+      <c r="BD8" s="10"/>
+      <c r="BE8" s="10"/>
+      <c r="BF8" s="10"/>
+      <c r="BG8" s="10"/>
+      <c r="BH8" s="10"/>
+      <c r="BI8" s="10"/>
+      <c r="BJ8" s="10"/>
+      <c r="BK8" s="10"/>
+      <c r="BL8" s="10"/>
+      <c r="BM8" s="10"/>
+      <c r="BN8" s="10"/>
+      <c r="BO8" s="10"/>
+      <c r="BP8" s="10"/>
+      <c r="BQ8" s="10"/>
+      <c r="BR8" s="10"/>
+      <c r="BS8" s="10"/>
+      <c r="BT8" s="10"/>
+      <c r="BU8" s="10"/>
+      <c r="BV8" s="10"/>
+      <c r="BW8" s="10"/>
+      <c r="BX8" s="10"/>
+      <c r="BY8" s="10"/>
+      <c r="BZ8" s="10"/>
+      <c r="CA8" s="10"/>
+      <c r="CB8" s="10"/>
+      <c r="CC8" s="10"/>
+      <c r="CD8" s="10"/>
+      <c r="CE8" s="10"/>
+      <c r="CF8" s="10"/>
+      <c r="CG8" s="10"/>
+      <c r="CH8" s="10"/>
+      <c r="CI8" s="10"/>
+      <c r="CJ8" s="10"/>
+      <c r="CK8" s="10"/>
+      <c r="CL8" s="10"/>
+      <c r="CM8" s="10"/>
+      <c r="CN8" s="10"/>
+      <c r="CO8" s="10"/>
+      <c r="CP8" s="10"/>
+      <c r="CQ8" s="10"/>
+      <c r="CR8" s="10"/>
+      <c r="CS8" s="10"/>
+      <c r="CT8" s="10"/>
+      <c r="CU8" s="10"/>
+      <c r="CV8" s="10"/>
+      <c r="CW8" s="10"/>
+      <c r="CX8" s="10"/>
+      <c r="CY8" s="10"/>
+      <c r="CZ8" s="10"/>
+      <c r="DA8" s="10"/>
+      <c r="DB8" s="10"/>
+      <c r="DC8" s="10"/>
+      <c r="DD8" s="10"/>
+    </row>
+    <row r="9" spans="1:108" x14ac:dyDescent="0.25">
+      <c r="N9" s="9"/>
+      <c r="O9" s="10"/>
+      <c r="P9" s="10"/>
+      <c r="Q9" s="10"/>
+      <c r="R9" s="10"/>
+      <c r="S9" s="10"/>
+      <c r="T9" s="10"/>
+      <c r="U9" s="10"/>
+      <c r="V9" s="10"/>
+      <c r="W9" s="10"/>
+      <c r="X9" s="10"/>
+      <c r="Y9" s="10"/>
+      <c r="Z9" s="10"/>
+      <c r="AA9" s="10"/>
+      <c r="AB9" s="10"/>
+      <c r="AC9" s="10"/>
+      <c r="AD9" s="10"/>
+      <c r="AE9" s="10"/>
+      <c r="AF9" s="10"/>
+      <c r="AG9" s="10"/>
+      <c r="AH9" s="10"/>
+      <c r="AI9" s="10"/>
+      <c r="AJ9" s="10"/>
+      <c r="AK9" s="10"/>
+      <c r="AL9" s="10"/>
+      <c r="AM9" s="10"/>
+      <c r="AN9" s="10"/>
+      <c r="AO9" s="10"/>
+      <c r="AP9" s="10"/>
+      <c r="AQ9" s="10"/>
+      <c r="AR9" s="10"/>
+      <c r="AS9" s="10"/>
+      <c r="AT9" s="10"/>
+      <c r="AU9" s="10"/>
+      <c r="AV9" s="10"/>
+      <c r="AW9" s="10"/>
+      <c r="AX9" s="10"/>
+      <c r="AY9" s="10"/>
+      <c r="AZ9" s="10"/>
+      <c r="BA9" s="10"/>
+      <c r="BB9" s="10"/>
+      <c r="BC9" s="10"/>
+      <c r="BD9" s="10"/>
+      <c r="BE9" s="10"/>
+      <c r="BF9" s="10"/>
+      <c r="BG9" s="10"/>
+      <c r="BH9" s="10"/>
+      <c r="BI9" s="10"/>
+      <c r="BJ9" s="10"/>
+      <c r="BK9" s="10"/>
+      <c r="BL9" s="10"/>
+      <c r="BM9" s="10"/>
+      <c r="BN9" s="10"/>
+      <c r="BO9" s="10"/>
+      <c r="BP9" s="10"/>
+      <c r="BQ9" s="10"/>
+      <c r="BR9" s="10"/>
+      <c r="BS9" s="10"/>
+      <c r="BT9" s="10"/>
+      <c r="BU9" s="10"/>
+      <c r="BV9" s="10"/>
+      <c r="BW9" s="10"/>
+      <c r="BX9" s="10"/>
+      <c r="BY9" s="10"/>
+      <c r="BZ9" s="10"/>
+      <c r="CA9" s="10"/>
+      <c r="CB9" s="10"/>
+      <c r="CC9" s="10"/>
+      <c r="CD9" s="10"/>
+      <c r="CE9" s="10"/>
+      <c r="CF9" s="10"/>
+      <c r="CG9" s="10"/>
+      <c r="CH9" s="10"/>
+      <c r="CI9" s="10"/>
+      <c r="CJ9" s="10"/>
+      <c r="CK9" s="10"/>
+      <c r="CL9" s="10"/>
+      <c r="CM9" s="10"/>
+      <c r="CN9" s="10"/>
+      <c r="CO9" s="10"/>
+      <c r="CP9" s="10"/>
+      <c r="CQ9" s="10"/>
+      <c r="CR9" s="10"/>
+      <c r="CS9" s="10"/>
+      <c r="CT9" s="10"/>
+      <c r="CU9" s="10"/>
+      <c r="CV9" s="10"/>
+      <c r="CW9" s="10"/>
+      <c r="CX9" s="10"/>
+      <c r="CY9" s="10"/>
+      <c r="CZ9" s="10"/>
+      <c r="DA9" s="10"/>
+      <c r="DB9" s="10"/>
+      <c r="DC9" s="10"/>
+      <c r="DD9" s="10"/>
+    </row>
+    <row r="10" spans="1:108" x14ac:dyDescent="0.25">
+      <c r="N10" s="9"/>
+      <c r="O10" s="10"/>
+      <c r="P10" s="10"/>
+      <c r="Q10" s="10"/>
+      <c r="R10" s="10"/>
+      <c r="S10" s="10"/>
+      <c r="T10" s="10"/>
+      <c r="U10" s="10"/>
+      <c r="V10" s="10"/>
+      <c r="W10" s="10"/>
+      <c r="X10" s="10"/>
+      <c r="Y10" s="10"/>
+      <c r="Z10" s="10"/>
+      <c r="AA10" s="10"/>
+      <c r="AB10" s="10"/>
+      <c r="AC10" s="10"/>
+      <c r="AD10" s="10"/>
+      <c r="AE10" s="10"/>
+      <c r="AF10" s="10"/>
+      <c r="AG10" s="10"/>
+      <c r="AH10" s="10"/>
+      <c r="AI10" s="10"/>
+      <c r="AJ10" s="10"/>
+      <c r="AK10" s="10"/>
+      <c r="AL10" s="10"/>
+      <c r="AM10" s="10"/>
+      <c r="AN10" s="10"/>
+      <c r="AO10" s="10"/>
+      <c r="AP10" s="10"/>
+      <c r="AQ10" s="10"/>
+      <c r="AR10" s="10"/>
+      <c r="AS10" s="10"/>
+      <c r="AT10" s="10"/>
+      <c r="AU10" s="10"/>
+      <c r="AV10" s="10"/>
+      <c r="AW10" s="10"/>
+      <c r="AX10" s="10"/>
+      <c r="AY10" s="10"/>
+      <c r="AZ10" s="10"/>
+      <c r="BA10" s="10"/>
+      <c r="BB10" s="10"/>
+      <c r="BC10" s="10"/>
+      <c r="BD10" s="10"/>
+      <c r="BE10" s="10"/>
+      <c r="BF10" s="10"/>
+      <c r="BG10" s="10"/>
+      <c r="BH10" s="10"/>
+      <c r="BI10" s="10"/>
+      <c r="BJ10" s="10"/>
+      <c r="BK10" s="10"/>
+      <c r="BL10" s="10"/>
+      <c r="BM10" s="10"/>
+      <c r="BN10" s="10"/>
+      <c r="BO10" s="10"/>
+      <c r="BP10" s="10"/>
+      <c r="BQ10" s="10"/>
+      <c r="BR10" s="10"/>
+      <c r="BS10" s="10"/>
+      <c r="BT10" s="10"/>
+      <c r="BU10" s="10"/>
+      <c r="BV10" s="10"/>
+      <c r="BW10" s="10"/>
+      <c r="BX10" s="10"/>
+      <c r="BY10" s="10"/>
+      <c r="BZ10" s="10"/>
+      <c r="CA10" s="10"/>
+      <c r="CB10" s="10"/>
+      <c r="CC10" s="10"/>
+      <c r="CD10" s="10"/>
+      <c r="CE10" s="10"/>
+      <c r="CF10" s="10"/>
+      <c r="CG10" s="10"/>
+      <c r="CH10" s="10"/>
+      <c r="CI10" s="10"/>
+      <c r="CJ10" s="10"/>
+      <c r="CK10" s="10"/>
+      <c r="CL10" s="10"/>
+      <c r="CM10" s="10"/>
+      <c r="CN10" s="10"/>
+      <c r="CO10" s="10"/>
+      <c r="CP10" s="10"/>
+      <c r="CQ10" s="10"/>
+      <c r="CR10" s="10"/>
+      <c r="CS10" s="10"/>
+      <c r="CT10" s="10"/>
+      <c r="CU10" s="10"/>
+      <c r="CV10" s="10"/>
+      <c r="CW10" s="10"/>
+      <c r="CX10" s="10"/>
+      <c r="CY10" s="10"/>
+      <c r="CZ10" s="10"/>
+      <c r="DA10" s="10"/>
+      <c r="DB10" s="10"/>
+      <c r="DC10" s="10"/>
+      <c r="DD10" s="10"/>
+    </row>
+    <row r="11" spans="1:108" x14ac:dyDescent="0.25">
+      <c r="N11" s="9"/>
+      <c r="O11" s="10"/>
+      <c r="P11" s="10"/>
+      <c r="Q11" s="10"/>
+      <c r="R11" s="10"/>
+      <c r="S11" s="10"/>
+      <c r="T11" s="10"/>
+      <c r="U11" s="10"/>
+      <c r="V11" s="10"/>
+      <c r="W11" s="10"/>
+      <c r="X11" s="10"/>
+      <c r="Y11" s="10"/>
+      <c r="Z11" s="10"/>
+      <c r="AA11" s="10"/>
+      <c r="AB11" s="10"/>
+      <c r="AC11" s="10"/>
+      <c r="AD11" s="10"/>
+      <c r="AE11" s="10"/>
+      <c r="AF11" s="10"/>
+      <c r="AG11" s="10"/>
+      <c r="AH11" s="10"/>
+      <c r="AI11" s="10"/>
+      <c r="AJ11" s="10"/>
+      <c r="AK11" s="10"/>
+      <c r="AL11" s="10"/>
+      <c r="AM11" s="10"/>
+      <c r="AN11" s="10"/>
+      <c r="AO11" s="10"/>
+      <c r="AP11" s="10"/>
+      <c r="AQ11" s="10"/>
+      <c r="AR11" s="10"/>
+      <c r="AS11" s="10"/>
+      <c r="AT11" s="10"/>
+      <c r="AU11" s="10"/>
+      <c r="AV11" s="10"/>
+      <c r="AW11" s="10"/>
+      <c r="AX11" s="10"/>
+      <c r="AY11" s="10"/>
+      <c r="AZ11" s="10"/>
+      <c r="BA11" s="10"/>
+      <c r="BB11" s="10"/>
+      <c r="BC11" s="10"/>
+      <c r="BD11" s="10"/>
+      <c r="BE11" s="10"/>
+      <c r="BF11" s="10"/>
+      <c r="BG11" s="10"/>
+      <c r="BH11" s="10"/>
+      <c r="BI11" s="10"/>
+      <c r="BJ11" s="10"/>
+      <c r="BK11" s="10"/>
+      <c r="BL11" s="10"/>
+      <c r="BM11" s="10"/>
+      <c r="BN11" s="10"/>
+      <c r="BO11" s="10"/>
+      <c r="BP11" s="10"/>
+      <c r="BQ11" s="10"/>
+      <c r="BR11" s="10"/>
+      <c r="BS11" s="10"/>
+      <c r="BT11" s="10"/>
+      <c r="BU11" s="10"/>
+      <c r="BV11" s="10"/>
+      <c r="BW11" s="10"/>
+      <c r="BX11" s="10"/>
+      <c r="BY11" s="10"/>
+      <c r="BZ11" s="10"/>
+      <c r="CA11" s="10"/>
+      <c r="CB11" s="10"/>
+      <c r="CC11" s="10"/>
+      <c r="CD11" s="10"/>
+      <c r="CE11" s="10"/>
+      <c r="CF11" s="10"/>
+      <c r="CG11" s="10"/>
+      <c r="CH11" s="10"/>
+      <c r="CI11" s="10"/>
+      <c r="CJ11" s="10"/>
+      <c r="CK11" s="10"/>
+      <c r="CL11" s="10"/>
+      <c r="CM11" s="10"/>
+      <c r="CN11" s="10"/>
+      <c r="CO11" s="10"/>
+      <c r="CP11" s="10"/>
+      <c r="CQ11" s="10"/>
+      <c r="CR11" s="10"/>
+      <c r="CS11" s="10"/>
+      <c r="CT11" s="10"/>
+      <c r="CU11" s="10"/>
+      <c r="CV11" s="10"/>
+      <c r="CW11" s="10"/>
+      <c r="CX11" s="10"/>
+      <c r="CY11" s="10"/>
+      <c r="CZ11" s="10"/>
+      <c r="DA11" s="10"/>
+      <c r="DB11" s="10"/>
+      <c r="DC11" s="10"/>
+      <c r="DD11" s="10"/>
+    </row>
+    <row r="12" spans="1:108" x14ac:dyDescent="0.25">
+      <c r="N12" s="9"/>
+      <c r="O12" s="10"/>
+      <c r="P12" s="10"/>
+      <c r="Q12" s="10"/>
+      <c r="R12" s="10"/>
+      <c r="S12" s="10"/>
+      <c r="T12" s="10"/>
+      <c r="U12" s="10"/>
+      <c r="V12" s="10"/>
+      <c r="W12" s="10"/>
+      <c r="X12" s="10"/>
+      <c r="Y12" s="10"/>
+      <c r="Z12" s="10"/>
+      <c r="AA12" s="10"/>
+      <c r="AB12" s="10"/>
+      <c r="AC12" s="10"/>
+      <c r="AD12" s="10"/>
+      <c r="AE12" s="10"/>
+      <c r="AF12" s="10"/>
+      <c r="AG12" s="10"/>
+      <c r="AH12" s="10"/>
+      <c r="AI12" s="10"/>
+      <c r="AJ12" s="10"/>
+      <c r="AK12" s="10"/>
+      <c r="AL12" s="10"/>
+      <c r="AM12" s="10"/>
+      <c r="AN12" s="10"/>
+      <c r="AO12" s="10"/>
+      <c r="AP12" s="10"/>
+      <c r="AQ12" s="10"/>
+      <c r="AR12" s="10"/>
+      <c r="AS12" s="10"/>
+      <c r="AT12" s="10"/>
+      <c r="AU12" s="10"/>
+      <c r="AV12" s="10"/>
+      <c r="AW12" s="10"/>
+      <c r="AX12" s="10"/>
+      <c r="AY12" s="10"/>
+      <c r="AZ12" s="10"/>
+      <c r="BA12" s="10"/>
+      <c r="BB12" s="10"/>
+      <c r="BC12" s="10"/>
+      <c r="BD12" s="10"/>
+      <c r="BE12" s="10"/>
+      <c r="BF12" s="10"/>
+      <c r="BG12" s="10"/>
+      <c r="BH12" s="10"/>
+      <c r="BI12" s="10"/>
+      <c r="BJ12" s="10"/>
+      <c r="BK12" s="10"/>
+      <c r="BL12" s="10"/>
+      <c r="BM12" s="10"/>
+      <c r="BN12" s="10"/>
+      <c r="BO12" s="10"/>
+      <c r="BP12" s="10"/>
+      <c r="BQ12" s="10"/>
+      <c r="BR12" s="10"/>
+      <c r="BS12" s="10"/>
+      <c r="BT12" s="10"/>
+      <c r="BU12" s="10"/>
+      <c r="BV12" s="10"/>
+      <c r="BW12" s="10"/>
+      <c r="BX12" s="10"/>
+      <c r="BY12" s="10"/>
+      <c r="BZ12" s="10"/>
+      <c r="CA12" s="10"/>
+      <c r="CB12" s="10"/>
+      <c r="CC12" s="10"/>
+      <c r="CD12" s="10"/>
+      <c r="CE12" s="10"/>
+      <c r="CF12" s="10"/>
+      <c r="CG12" s="10"/>
+      <c r="CH12" s="10"/>
+      <c r="CI12" s="10"/>
+      <c r="CJ12" s="10"/>
+      <c r="CK12" s="10"/>
+      <c r="CL12" s="10"/>
+      <c r="CM12" s="10"/>
+      <c r="CN12" s="10"/>
+      <c r="CO12" s="10"/>
+      <c r="CP12" s="10"/>
+      <c r="CQ12" s="10"/>
+      <c r="CR12" s="10"/>
+      <c r="CS12" s="10"/>
+      <c r="CT12" s="10"/>
+      <c r="CU12" s="10"/>
+      <c r="CV12" s="10"/>
+      <c r="CW12" s="10"/>
+      <c r="CX12" s="10"/>
+      <c r="CY12" s="10"/>
+      <c r="CZ12" s="10"/>
+      <c r="DA12" s="10"/>
+      <c r="DB12" s="10"/>
+      <c r="DC12" s="10"/>
+      <c r="DD12" s="10"/>
+    </row>
+    <row r="13" spans="1:108" x14ac:dyDescent="0.25">
+      <c r="N13" s="9"/>
+      <c r="O13" s="10"/>
+      <c r="P13" s="10"/>
+      <c r="Q13" s="10"/>
+      <c r="R13" s="10"/>
+      <c r="S13" s="10"/>
+      <c r="T13" s="10"/>
+      <c r="U13" s="10"/>
+      <c r="V13" s="10"/>
+      <c r="W13" s="10"/>
+      <c r="X13" s="10"/>
+      <c r="Y13" s="10"/>
+      <c r="Z13" s="10"/>
+      <c r="AA13" s="10"/>
+      <c r="AB13" s="10"/>
+      <c r="AC13" s="10"/>
+      <c r="AD13" s="10"/>
+      <c r="AE13" s="10"/>
+      <c r="AF13" s="10"/>
+      <c r="AG13" s="10"/>
+      <c r="AH13" s="10"/>
+      <c r="AI13" s="10"/>
+      <c r="AJ13" s="10"/>
+      <c r="AK13" s="10"/>
+      <c r="AL13" s="10"/>
+      <c r="AM13" s="10"/>
+      <c r="AN13" s="10"/>
+      <c r="AO13" s="10"/>
+      <c r="AP13" s="10"/>
+      <c r="AQ13" s="10"/>
+      <c r="AR13" s="10"/>
+      <c r="AS13" s="10"/>
+      <c r="AT13" s="10"/>
+      <c r="AU13" s="10"/>
+      <c r="AV13" s="10"/>
+      <c r="AW13" s="10"/>
+      <c r="AX13" s="10"/>
+      <c r="AY13" s="10"/>
+      <c r="AZ13" s="10"/>
+      <c r="BA13" s="10"/>
+      <c r="BB13" s="10"/>
+      <c r="BC13" s="10"/>
+      <c r="BD13" s="10"/>
+      <c r="BE13" s="10"/>
+      <c r="BF13" s="10"/>
+      <c r="BG13" s="10"/>
+      <c r="BH13" s="10"/>
+      <c r="BI13" s="10"/>
+      <c r="BJ13" s="10"/>
+      <c r="BK13" s="10"/>
+      <c r="BL13" s="10"/>
+      <c r="BM13" s="10"/>
+      <c r="BN13" s="10"/>
+      <c r="BO13" s="10"/>
+      <c r="BP13" s="10"/>
+      <c r="BQ13" s="10"/>
+      <c r="BR13" s="10"/>
+      <c r="BS13" s="10"/>
+      <c r="BT13" s="10"/>
+      <c r="BU13" s="10"/>
+      <c r="BV13" s="10"/>
+      <c r="BW13" s="10"/>
+      <c r="BX13" s="10"/>
+      <c r="BY13" s="10"/>
+      <c r="BZ13" s="10"/>
+      <c r="CA13" s="10"/>
+      <c r="CB13" s="10"/>
+      <c r="CC13" s="10"/>
+      <c r="CD13" s="10"/>
+      <c r="CE13" s="10"/>
+      <c r="CF13" s="10"/>
+      <c r="CG13" s="10"/>
+      <c r="CH13" s="10"/>
+      <c r="CI13" s="10"/>
+      <c r="CJ13" s="10"/>
+      <c r="CK13" s="10"/>
+      <c r="CL13" s="10"/>
+      <c r="CM13" s="10"/>
+      <c r="CN13" s="10"/>
+      <c r="CO13" s="10"/>
+      <c r="CP13" s="10"/>
+      <c r="CQ13" s="10"/>
+      <c r="CR13" s="10"/>
+      <c r="CS13" s="10"/>
+      <c r="CT13" s="10"/>
+      <c r="CU13" s="10"/>
+      <c r="CV13" s="10"/>
+      <c r="CW13" s="10"/>
+      <c r="CX13" s="10"/>
+      <c r="CY13" s="10"/>
+      <c r="CZ13" s="10"/>
+      <c r="DA13" s="10"/>
+      <c r="DB13" s="10"/>
+      <c r="DC13" s="10"/>
+      <c r="DD13" s="10"/>
+    </row>
+    <row r="14" spans="1:108" x14ac:dyDescent="0.25">
+      <c r="N14" s="9"/>
+      <c r="O14" s="10"/>
+      <c r="P14" s="10"/>
+      <c r="Q14" s="10"/>
+      <c r="R14" s="10"/>
+      <c r="S14" s="10"/>
+      <c r="T14" s="10"/>
+      <c r="U14" s="10"/>
+      <c r="V14" s="10"/>
+      <c r="W14" s="10"/>
+      <c r="X14" s="10"/>
+      <c r="Y14" s="10"/>
+      <c r="Z14" s="10"/>
+      <c r="AA14" s="10"/>
+      <c r="AB14" s="10"/>
+      <c r="AC14" s="10"/>
+      <c r="AD14" s="10"/>
+      <c r="AE14" s="10"/>
+      <c r="AF14" s="10"/>
+      <c r="AG14" s="10"/>
+      <c r="AH14" s="10"/>
+      <c r="AI14" s="10"/>
+      <c r="AJ14" s="10"/>
+      <c r="AK14" s="10"/>
+      <c r="AL14" s="10"/>
+      <c r="AM14" s="10"/>
+      <c r="AN14" s="10"/>
+      <c r="AO14" s="10"/>
+      <c r="AP14" s="10"/>
+      <c r="AQ14" s="10"/>
+      <c r="AR14" s="10"/>
+      <c r="AS14" s="10"/>
+      <c r="AT14" s="10"/>
+      <c r="AU14" s="10"/>
+      <c r="AV14" s="10"/>
+      <c r="AW14" s="10"/>
+      <c r="AX14" s="10"/>
+      <c r="AY14" s="10"/>
+      <c r="AZ14" s="10"/>
+      <c r="BA14" s="10"/>
+      <c r="BB14" s="10"/>
+      <c r="BC14" s="10"/>
+      <c r="BD14" s="10"/>
+      <c r="BE14" s="10"/>
+      <c r="BF14" s="10"/>
+      <c r="BG14" s="10"/>
+      <c r="BH14" s="10"/>
+      <c r="BI14" s="10"/>
+      <c r="BJ14" s="10"/>
+      <c r="BK14" s="10"/>
+      <c r="BL14" s="10"/>
+      <c r="BM14" s="10"/>
+      <c r="BN14" s="10"/>
+      <c r="BO14" s="10"/>
+      <c r="BP14" s="10"/>
+      <c r="BQ14" s="10"/>
+      <c r="BR14" s="10"/>
+      <c r="BS14" s="10"/>
+      <c r="BT14" s="10"/>
+      <c r="BU14" s="10"/>
+      <c r="BV14" s="10"/>
+      <c r="BW14" s="10"/>
+      <c r="BX14" s="10"/>
+      <c r="BY14" s="10"/>
+      <c r="BZ14" s="10"/>
+      <c r="CA14" s="10"/>
+      <c r="CB14" s="10"/>
+      <c r="CC14" s="10"/>
+      <c r="CD14" s="10"/>
+      <c r="CE14" s="10"/>
+      <c r="CF14" s="10"/>
+      <c r="CG14" s="10"/>
+      <c r="CH14" s="10"/>
+      <c r="CI14" s="10"/>
+      <c r="CJ14" s="10"/>
+      <c r="CK14" s="10"/>
+      <c r="CL14" s="10"/>
+      <c r="CM14" s="10"/>
+      <c r="CN14" s="10"/>
+      <c r="CO14" s="10"/>
+      <c r="CP14" s="10"/>
+      <c r="CQ14" s="10"/>
+      <c r="CR14" s="10"/>
+      <c r="CS14" s="10"/>
+      <c r="CT14" s="10"/>
+      <c r="CU14" s="10"/>
+      <c r="CV14" s="10"/>
+      <c r="CW14" s="10"/>
+      <c r="CX14" s="10"/>
+      <c r="CY14" s="10"/>
+      <c r="CZ14" s="10"/>
+      <c r="DA14" s="10"/>
+      <c r="DB14" s="10"/>
+      <c r="DC14" s="10"/>
+      <c r="DD14" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="B2:G2"/>
+    <mergeCell ref="A2:M2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>